<commit_message>
ppp total concentration plot
</commit_message>
<xml_diff>
--- a/01_input/ppp_results_florian_final_2025_02_07.xlsx
+++ b/01_input/ppp_results_florian_final_2025_02_07.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucnmuni-my.sharepoint.com/personal/150537_muni_cz/Documents/Plocha/Rcx/6_Analytika/Stážisti/Výsledky/2025_01_Florian/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f304f79f068e311c/Universitaet/MASTER/MasterThesis/11_Data_Analysis_MA/01_input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="83" documentId="8_{4906466F-4855-49E0-A53F-BB0CA239825D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{642FBCBF-4668-4AED-B1B8-8AA3BBBB0D60}"/>
+  <xr:revisionPtr revIDLastSave="85" documentId="8_{4906466F-4855-49E0-A53F-BB0CA239825D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B84AF89-1641-4362-8239-8B36E209FA84}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="positive" sheetId="1" r:id="rId1"/>
@@ -1144,8 +1144,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
     <cellStyle name="Normální 2" xfId="1" xr:uid="{8A6B3E42-3139-40EE-BAB5-350146CD222C}"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -6965,20 +6965,24 @@
   <dimension ref="A1:ES37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="DG4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="BQ4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="BM32" sqref="BM32:BM33"/>
+      <selection pane="bottomRight" activeCell="BQ1" sqref="BQ1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="11" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="2" customWidth="1"/>
-    <col min="2" max="149" width="6.42578125" style="2" customWidth="1"/>
-    <col min="150" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="12.54296875" style="2" customWidth="1"/>
+    <col min="2" max="54" width="6.40625" style="2" customWidth="1"/>
+    <col min="55" max="55" width="18" style="2" customWidth="1"/>
+    <col min="56" max="68" width="6.40625" style="2" customWidth="1"/>
+    <col min="69" max="69" width="39.26953125" style="2" customWidth="1"/>
+    <col min="70" max="149" width="6.40625" style="2" customWidth="1"/>
+    <col min="150" max="16384" width="9.1328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:149" s="11" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:149" s="11" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -7427,7 +7431,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="2" spans="1:149" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:149" ht="12" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A2" s="4" t="s">
         <v>156</v>
       </c>
@@ -7876,7 +7880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:149" x14ac:dyDescent="0.6">
       <c r="A3" s="6" t="s">
         <v>10</v>
       </c>
@@ -8325,7 +8329,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="4" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:149" x14ac:dyDescent="0.6">
       <c r="A4" s="6" t="s">
         <v>16</v>
       </c>
@@ -8774,7 +8778,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="5" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:149" x14ac:dyDescent="0.6">
       <c r="A5" s="6" t="s">
         <v>26</v>
       </c>
@@ -9223,7 +9227,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="6" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:149" x14ac:dyDescent="0.6">
       <c r="A6" s="6" t="s">
         <v>25</v>
       </c>
@@ -9672,7 +9676,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="7" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:149" x14ac:dyDescent="0.6">
       <c r="A7" s="6" t="s">
         <v>30</v>
       </c>
@@ -10121,7 +10125,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:149" x14ac:dyDescent="0.6">
       <c r="A8" s="6" t="s">
         <v>9</v>
       </c>
@@ -10570,7 +10574,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="9" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:149" x14ac:dyDescent="0.6">
       <c r="A9" s="6" t="s">
         <v>19</v>
       </c>
@@ -11019,7 +11023,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="10" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:149" x14ac:dyDescent="0.6">
       <c r="A10" s="6" t="s">
         <v>34</v>
       </c>
@@ -11468,7 +11472,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="11" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:149" x14ac:dyDescent="0.6">
       <c r="A11" s="6" t="s">
         <v>5</v>
       </c>
@@ -11917,7 +11921,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:149" x14ac:dyDescent="0.6">
       <c r="A12" s="6" t="s">
         <v>28</v>
       </c>
@@ -12366,7 +12370,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="13" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:149" x14ac:dyDescent="0.6">
       <c r="A13" s="6" t="s">
         <v>4</v>
       </c>
@@ -12815,7 +12819,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="14" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:149" x14ac:dyDescent="0.6">
       <c r="A14" s="6" t="s">
         <v>36</v>
       </c>
@@ -13264,7 +13268,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="15" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:149" x14ac:dyDescent="0.6">
       <c r="A15" s="6" t="s">
         <v>6</v>
       </c>
@@ -13713,7 +13717,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="16" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:149" x14ac:dyDescent="0.6">
       <c r="A16" s="6" t="s">
         <v>29</v>
       </c>
@@ -14162,7 +14166,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="17" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:149" x14ac:dyDescent="0.6">
       <c r="A17" s="6" t="s">
         <v>24</v>
       </c>
@@ -14611,7 +14615,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="18" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:149" x14ac:dyDescent="0.6">
       <c r="A18" s="6" t="s">
         <v>31</v>
       </c>
@@ -15060,7 +15064,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="19" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:149" x14ac:dyDescent="0.6">
       <c r="A19" s="6" t="s">
         <v>33</v>
       </c>
@@ -15509,7 +15513,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="20" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:149" x14ac:dyDescent="0.6">
       <c r="A20" s="6" t="s">
         <v>27</v>
       </c>
@@ -15958,7 +15962,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="21" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:149" x14ac:dyDescent="0.6">
       <c r="A21" s="6" t="s">
         <v>22</v>
       </c>
@@ -16407,7 +16411,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="22" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:149" x14ac:dyDescent="0.6">
       <c r="A22" s="6" t="s">
         <v>17</v>
       </c>
@@ -16856,7 +16860,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="23" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:149" x14ac:dyDescent="0.6">
       <c r="A23" s="6" t="s">
         <v>20</v>
       </c>
@@ -17305,7 +17309,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="24" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:149" x14ac:dyDescent="0.6">
       <c r="A24" s="6" t="s">
         <v>8</v>
       </c>
@@ -17754,7 +17758,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="25" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:149" x14ac:dyDescent="0.6">
       <c r="A25" s="6" t="s">
         <v>0</v>
       </c>
@@ -18203,7 +18207,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="26" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:149" x14ac:dyDescent="0.6">
       <c r="A26" s="6" t="s">
         <v>23</v>
       </c>
@@ -18652,7 +18656,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="27" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:149" x14ac:dyDescent="0.6">
       <c r="A27" s="6" t="s">
         <v>1</v>
       </c>
@@ -19101,7 +19105,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="28" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:149" x14ac:dyDescent="0.6">
       <c r="A28" s="6" t="s">
         <v>37</v>
       </c>
@@ -19550,7 +19554,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="29" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:149" x14ac:dyDescent="0.6">
       <c r="A29" s="6" t="s">
         <v>21</v>
       </c>
@@ -19999,7 +20003,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="30" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:149" x14ac:dyDescent="0.6">
       <c r="A30" s="6" t="s">
         <v>35</v>
       </c>
@@ -20448,7 +20452,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="31" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:149" x14ac:dyDescent="0.6">
       <c r="A31" s="6" t="s">
         <v>3</v>
       </c>
@@ -20897,7 +20901,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="32" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:149" x14ac:dyDescent="0.6">
       <c r="A32" s="6" t="s">
         <v>15</v>
       </c>
@@ -21346,7 +21350,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="33" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:149" x14ac:dyDescent="0.6">
       <c r="A33" s="6" t="s">
         <v>13</v>
       </c>
@@ -21795,7 +21799,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="34" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:149" x14ac:dyDescent="0.6">
       <c r="A34" s="6" t="s">
         <v>14</v>
       </c>
@@ -22244,7 +22248,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="35" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:149" x14ac:dyDescent="0.6">
       <c r="A35" s="6" t="s">
         <v>32</v>
       </c>
@@ -22693,7 +22697,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="36" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:149" x14ac:dyDescent="0.6">
       <c r="A36" s="6" t="s">
         <v>2</v>
       </c>
@@ -23142,7 +23146,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="37" spans="1:149" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:149" x14ac:dyDescent="0.6">
       <c r="A37" s="6" t="s">
         <v>11</v>
       </c>
@@ -23612,14 +23616,14 @@
       <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="11" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="5" customWidth="1"/>
-    <col min="2" max="16" width="7.7109375" style="5" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="12.40625" style="5" customWidth="1"/>
+    <col min="2" max="16" width="7.7265625" style="5" customWidth="1"/>
+    <col min="17" max="16384" width="9.1328125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
@@ -23669,7 +23673,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A2" s="4" t="s">
         <v>157</v>
       </c>
@@ -23719,7 +23723,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A3" s="10" t="s">
         <v>156</v>
       </c>
@@ -23769,7 +23773,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.6">
       <c r="A4" s="6" t="s">
         <v>55</v>
       </c>
@@ -23819,7 +23823,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.6">
       <c r="A5" s="6" t="s">
         <v>56</v>
       </c>
@@ -23869,7 +23873,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.6">
       <c r="A6" s="6" t="s">
         <v>57</v>
       </c>
@@ -23919,7 +23923,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.6">
       <c r="A7" s="6" t="s">
         <v>58</v>
       </c>
@@ -23969,7 +23973,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.6">
       <c r="A8" s="6" t="s">
         <v>59</v>
       </c>
@@ -24019,7 +24023,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.6">
       <c r="A9" s="6" t="s">
         <v>60</v>
       </c>
@@ -24069,7 +24073,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.6">
       <c r="A10" s="6" t="s">
         <v>61</v>
       </c>
@@ -24119,7 +24123,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.6">
       <c r="A11" s="6" t="s">
         <v>62</v>
       </c>
@@ -24169,7 +24173,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.6">
       <c r="A12" s="6" t="s">
         <v>63</v>
       </c>
@@ -24219,7 +24223,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.6">
       <c r="A13" s="6" t="s">
         <v>64</v>
       </c>
@@ -24269,7 +24273,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.6">
       <c r="A14" s="6" t="s">
         <v>65</v>
       </c>
@@ -24319,7 +24323,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.6">
       <c r="A15" s="6" t="s">
         <v>66</v>
       </c>
@@ -24369,7 +24373,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.6">
       <c r="A16" s="6" t="s">
         <v>67</v>
       </c>
@@ -24419,7 +24423,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.6">
       <c r="A17" s="6" t="s">
         <v>68</v>
       </c>
@@ -24469,7 +24473,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.6">
       <c r="A18" s="6" t="s">
         <v>69</v>
       </c>
@@ -24519,7 +24523,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.6">
       <c r="A19" s="6" t="s">
         <v>70</v>
       </c>
@@ -24569,7 +24573,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.6">
       <c r="A20" s="6" t="s">
         <v>71</v>
       </c>
@@ -24619,7 +24623,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.6">
       <c r="A21" s="6" t="s">
         <v>72</v>
       </c>
@@ -24669,7 +24673,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.6">
       <c r="A22" s="6" t="s">
         <v>73</v>
       </c>
@@ -24719,7 +24723,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.6">
       <c r="A23" s="6" t="s">
         <v>74</v>
       </c>
@@ -24769,7 +24773,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.6">
       <c r="A24" s="6" t="s">
         <v>75</v>
       </c>
@@ -24819,7 +24823,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.6">
       <c r="A25" s="6" t="s">
         <v>76</v>
       </c>
@@ -24869,7 +24873,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.6">
       <c r="A26" s="6" t="s">
         <v>77</v>
       </c>
@@ -24919,7 +24923,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.6">
       <c r="A27" s="6" t="s">
         <v>78</v>
       </c>
@@ -24969,7 +24973,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.6">
       <c r="A28" s="6" t="s">
         <v>79</v>
       </c>
@@ -25019,7 +25023,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.6">
       <c r="A29" s="6" t="s">
         <v>80</v>
       </c>
@@ -25069,7 +25073,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.6">
       <c r="A30" s="6" t="s">
         <v>81</v>
       </c>
@@ -25119,7 +25123,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.6">
       <c r="A31" s="6" t="s">
         <v>82</v>
       </c>
@@ -25169,7 +25173,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.6">
       <c r="A32" s="6" t="s">
         <v>83</v>
       </c>
@@ -25219,7 +25223,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.6">
       <c r="A33" s="6" t="s">
         <v>84</v>
       </c>
@@ -25269,7 +25273,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.6">
       <c r="A34" s="6" t="s">
         <v>85</v>
       </c>
@@ -25319,7 +25323,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.6">
       <c r="A35" s="6" t="s">
         <v>86</v>
       </c>
@@ -25369,7 +25373,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.6">
       <c r="A36" s="6" t="s">
         <v>87</v>
       </c>
@@ -25419,7 +25423,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.6">
       <c r="A37" s="6" t="s">
         <v>88</v>
       </c>
@@ -25469,7 +25473,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.6">
       <c r="A38" s="6" t="s">
         <v>89</v>
       </c>
@@ -25535,14 +25539,14 @@
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="11" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="5" customWidth="1"/>
-    <col min="2" max="3" width="6.85546875" style="5" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="10.86328125" style="5" customWidth="1"/>
+    <col min="2" max="3" width="6.86328125" style="5" customWidth="1"/>
+    <col min="4" max="16384" width="9.1328125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
@@ -25553,7 +25557,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A2" s="4" t="s">
         <v>18</v>
       </c>
@@ -25564,7 +25568,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A3" s="10"/>
       <c r="B3" s="10" t="s">
         <v>38</v>
@@ -25573,7 +25577,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A4" s="6" t="s">
         <v>92</v>
       </c>
@@ -25584,7 +25588,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A5" s="6" t="s">
         <v>93</v>
       </c>
@@ -25595,7 +25599,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A6" s="6" t="s">
         <v>94</v>
       </c>
@@ -25606,7 +25610,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A7" s="6" t="s">
         <v>95</v>
       </c>
@@ -25617,7 +25621,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A8" s="6" t="s">
         <v>96</v>
       </c>
@@ -25628,7 +25632,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A9" s="6" t="s">
         <v>97</v>
       </c>
@@ -25639,7 +25643,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A10" s="6" t="s">
         <v>98</v>
       </c>
@@ -25650,7 +25654,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A11" s="6" t="s">
         <v>99</v>
       </c>
@@ -25661,7 +25665,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A12" s="6" t="s">
         <v>100</v>
       </c>
@@ -25672,7 +25676,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A13" s="6" t="s">
         <v>101</v>
       </c>
@@ -25683,7 +25687,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A14" s="6" t="s">
         <v>102</v>
       </c>
@@ -25694,7 +25698,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A15" s="6" t="s">
         <v>103</v>
       </c>
@@ -25705,7 +25709,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A16" s="6" t="s">
         <v>104</v>
       </c>
@@ -25716,7 +25720,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A17" s="6" t="s">
         <v>105</v>
       </c>
@@ -25727,7 +25731,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A18" s="6" t="s">
         <v>106</v>
       </c>
@@ -25738,7 +25742,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A19" s="6" t="s">
         <v>107</v>
       </c>
@@ -25749,7 +25753,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A20" s="6" t="s">
         <v>108</v>
       </c>
@@ -25760,7 +25764,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A21" s="6" t="s">
         <v>109</v>
       </c>
@@ -25771,7 +25775,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A22" s="6" t="s">
         <v>110</v>
       </c>
@@ -25782,7 +25786,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A23" s="6" t="s">
         <v>111</v>
       </c>
@@ -25793,7 +25797,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A24" s="6" t="s">
         <v>112</v>
       </c>
@@ -25804,7 +25808,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A25" s="6" t="s">
         <v>113</v>
       </c>
@@ -25815,7 +25819,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A26" s="6" t="s">
         <v>114</v>
       </c>
@@ -25826,7 +25830,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A27" s="6" t="s">
         <v>115</v>
       </c>
@@ -25837,7 +25841,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A28" s="6" t="s">
         <v>116</v>
       </c>
@@ -25848,7 +25852,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A29" s="6" t="s">
         <v>117</v>
       </c>
@@ -25859,7 +25863,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A30" s="6" t="s">
         <v>118</v>
       </c>
@@ -25870,7 +25874,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A31" s="6" t="s">
         <v>119</v>
       </c>
@@ -25881,7 +25885,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A32" s="6" t="s">
         <v>120</v>
       </c>
@@ -25892,7 +25896,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A33" s="6" t="s">
         <v>121</v>
       </c>
@@ -25903,7 +25907,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A34" s="6" t="s">
         <v>122</v>
       </c>
@@ -25914,7 +25918,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A35" s="6" t="s">
         <v>123</v>
       </c>
@@ -25925,7 +25929,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A36" s="6" t="s">
         <v>124</v>
       </c>
@@ -25936,7 +25940,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A37" s="6" t="s">
         <v>125</v>
       </c>
@@ -25947,7 +25951,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A38" s="6" t="s">
         <v>126</v>
       </c>
@@ -25971,142 +25975,142 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="AE1" sqref="AE1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="13" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="256" width="8.7109375" style="13"/>
-    <col min="257" max="257" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="258" max="512" width="8.7109375" style="13"/>
-    <col min="513" max="513" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="514" max="768" width="8.7109375" style="13"/>
-    <col min="769" max="769" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="770" max="1024" width="8.7109375" style="13"/>
-    <col min="1025" max="1025" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="1026" max="1280" width="8.7109375" style="13"/>
-    <col min="1281" max="1281" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="1282" max="1536" width="8.7109375" style="13"/>
-    <col min="1537" max="1537" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="1538" max="1792" width="8.7109375" style="13"/>
-    <col min="1793" max="1793" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="1794" max="2048" width="8.7109375" style="13"/>
-    <col min="2049" max="2049" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="2050" max="2304" width="8.7109375" style="13"/>
-    <col min="2305" max="2305" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="2306" max="2560" width="8.7109375" style="13"/>
-    <col min="2561" max="2561" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="2562" max="2816" width="8.7109375" style="13"/>
-    <col min="2817" max="2817" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="2818" max="3072" width="8.7109375" style="13"/>
-    <col min="3073" max="3073" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="3074" max="3328" width="8.7109375" style="13"/>
-    <col min="3329" max="3329" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="3330" max="3584" width="8.7109375" style="13"/>
-    <col min="3585" max="3585" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="3586" max="3840" width="8.7109375" style="13"/>
-    <col min="3841" max="3841" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="3842" max="4096" width="8.7109375" style="13"/>
-    <col min="4097" max="4097" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4098" max="4352" width="8.7109375" style="13"/>
-    <col min="4353" max="4353" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4354" max="4608" width="8.7109375" style="13"/>
-    <col min="4609" max="4609" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4610" max="4864" width="8.7109375" style="13"/>
-    <col min="4865" max="4865" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4866" max="5120" width="8.7109375" style="13"/>
-    <col min="5121" max="5121" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="5122" max="5376" width="8.7109375" style="13"/>
-    <col min="5377" max="5377" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="5378" max="5632" width="8.7109375" style="13"/>
-    <col min="5633" max="5633" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="5634" max="5888" width="8.7109375" style="13"/>
-    <col min="5889" max="5889" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="5890" max="6144" width="8.7109375" style="13"/>
-    <col min="6145" max="6145" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="6146" max="6400" width="8.7109375" style="13"/>
-    <col min="6401" max="6401" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="6402" max="6656" width="8.7109375" style="13"/>
-    <col min="6657" max="6657" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="6658" max="6912" width="8.7109375" style="13"/>
-    <col min="6913" max="6913" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="6914" max="7168" width="8.7109375" style="13"/>
-    <col min="7169" max="7169" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="7170" max="7424" width="8.7109375" style="13"/>
-    <col min="7425" max="7425" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="7426" max="7680" width="8.7109375" style="13"/>
-    <col min="7681" max="7681" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="7682" max="7936" width="8.7109375" style="13"/>
-    <col min="7937" max="7937" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="7938" max="8192" width="8.7109375" style="13"/>
-    <col min="8193" max="8193" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="8194" max="8448" width="8.7109375" style="13"/>
-    <col min="8449" max="8449" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="8450" max="8704" width="8.7109375" style="13"/>
-    <col min="8705" max="8705" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="8706" max="8960" width="8.7109375" style="13"/>
-    <col min="8961" max="8961" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="8962" max="9216" width="8.7109375" style="13"/>
-    <col min="9217" max="9217" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="9218" max="9472" width="8.7109375" style="13"/>
-    <col min="9473" max="9473" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="9474" max="9728" width="8.7109375" style="13"/>
-    <col min="9729" max="9729" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="9730" max="9984" width="8.7109375" style="13"/>
-    <col min="9985" max="9985" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="9986" max="10240" width="8.7109375" style="13"/>
-    <col min="10241" max="10241" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="10242" max="10496" width="8.7109375" style="13"/>
-    <col min="10497" max="10497" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="10498" max="10752" width="8.7109375" style="13"/>
-    <col min="10753" max="10753" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="10754" max="11008" width="8.7109375" style="13"/>
-    <col min="11009" max="11009" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="11010" max="11264" width="8.7109375" style="13"/>
-    <col min="11265" max="11265" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="11266" max="11520" width="8.7109375" style="13"/>
-    <col min="11521" max="11521" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="11522" max="11776" width="8.7109375" style="13"/>
-    <col min="11777" max="11777" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="11778" max="12032" width="8.7109375" style="13"/>
-    <col min="12033" max="12033" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="12034" max="12288" width="8.7109375" style="13"/>
-    <col min="12289" max="12289" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="12290" max="12544" width="8.7109375" style="13"/>
-    <col min="12545" max="12545" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="12546" max="12800" width="8.7109375" style="13"/>
-    <col min="12801" max="12801" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="12802" max="13056" width="8.7109375" style="13"/>
-    <col min="13057" max="13057" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="13058" max="13312" width="8.7109375" style="13"/>
-    <col min="13313" max="13313" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="13314" max="13568" width="8.7109375" style="13"/>
-    <col min="13569" max="13569" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="13570" max="13824" width="8.7109375" style="13"/>
-    <col min="13825" max="13825" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="13826" max="14080" width="8.7109375" style="13"/>
-    <col min="14081" max="14081" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="14082" max="14336" width="8.7109375" style="13"/>
-    <col min="14337" max="14337" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="14338" max="14592" width="8.7109375" style="13"/>
-    <col min="14593" max="14593" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="14594" max="14848" width="8.7109375" style="13"/>
-    <col min="14849" max="14849" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="14850" max="15104" width="8.7109375" style="13"/>
-    <col min="15105" max="15105" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="15106" max="15360" width="8.7109375" style="13"/>
-    <col min="15361" max="15361" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="15362" max="15616" width="8.7109375" style="13"/>
-    <col min="15617" max="15617" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="15618" max="15872" width="8.7109375" style="13"/>
-    <col min="15873" max="15873" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="15874" max="16128" width="8.7109375" style="13"/>
-    <col min="16129" max="16129" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="16130" max="16384" width="8.7109375" style="13"/>
+    <col min="1" max="1" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="256" width="8.7265625" style="13"/>
+    <col min="257" max="257" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="258" max="512" width="8.7265625" style="13"/>
+    <col min="513" max="513" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="514" max="768" width="8.7265625" style="13"/>
+    <col min="769" max="769" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="770" max="1024" width="8.7265625" style="13"/>
+    <col min="1025" max="1025" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="1026" max="1280" width="8.7265625" style="13"/>
+    <col min="1281" max="1281" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="1282" max="1536" width="8.7265625" style="13"/>
+    <col min="1537" max="1537" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="1538" max="1792" width="8.7265625" style="13"/>
+    <col min="1793" max="1793" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="1794" max="2048" width="8.7265625" style="13"/>
+    <col min="2049" max="2049" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="2050" max="2304" width="8.7265625" style="13"/>
+    <col min="2305" max="2305" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="2306" max="2560" width="8.7265625" style="13"/>
+    <col min="2561" max="2561" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="2562" max="2816" width="8.7265625" style="13"/>
+    <col min="2817" max="2817" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="2818" max="3072" width="8.7265625" style="13"/>
+    <col min="3073" max="3073" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="3074" max="3328" width="8.7265625" style="13"/>
+    <col min="3329" max="3329" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="3330" max="3584" width="8.7265625" style="13"/>
+    <col min="3585" max="3585" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="3586" max="3840" width="8.7265625" style="13"/>
+    <col min="3841" max="3841" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="3842" max="4096" width="8.7265625" style="13"/>
+    <col min="4097" max="4097" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="4098" max="4352" width="8.7265625" style="13"/>
+    <col min="4353" max="4353" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="4354" max="4608" width="8.7265625" style="13"/>
+    <col min="4609" max="4609" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="4610" max="4864" width="8.7265625" style="13"/>
+    <col min="4865" max="4865" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="4866" max="5120" width="8.7265625" style="13"/>
+    <col min="5121" max="5121" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="5122" max="5376" width="8.7265625" style="13"/>
+    <col min="5377" max="5377" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="5378" max="5632" width="8.7265625" style="13"/>
+    <col min="5633" max="5633" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="5634" max="5888" width="8.7265625" style="13"/>
+    <col min="5889" max="5889" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="5890" max="6144" width="8.7265625" style="13"/>
+    <col min="6145" max="6145" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="6146" max="6400" width="8.7265625" style="13"/>
+    <col min="6401" max="6401" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="6402" max="6656" width="8.7265625" style="13"/>
+    <col min="6657" max="6657" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="6658" max="6912" width="8.7265625" style="13"/>
+    <col min="6913" max="6913" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="6914" max="7168" width="8.7265625" style="13"/>
+    <col min="7169" max="7169" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="7170" max="7424" width="8.7265625" style="13"/>
+    <col min="7425" max="7425" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="7426" max="7680" width="8.7265625" style="13"/>
+    <col min="7681" max="7681" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="7682" max="7936" width="8.7265625" style="13"/>
+    <col min="7937" max="7937" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="7938" max="8192" width="8.7265625" style="13"/>
+    <col min="8193" max="8193" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="8194" max="8448" width="8.7265625" style="13"/>
+    <col min="8449" max="8449" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="8450" max="8704" width="8.7265625" style="13"/>
+    <col min="8705" max="8705" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="8706" max="8960" width="8.7265625" style="13"/>
+    <col min="8961" max="8961" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="8962" max="9216" width="8.7265625" style="13"/>
+    <col min="9217" max="9217" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9218" max="9472" width="8.7265625" style="13"/>
+    <col min="9473" max="9473" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9474" max="9728" width="8.7265625" style="13"/>
+    <col min="9729" max="9729" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9730" max="9984" width="8.7265625" style="13"/>
+    <col min="9985" max="9985" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9986" max="10240" width="8.7265625" style="13"/>
+    <col min="10241" max="10241" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10242" max="10496" width="8.7265625" style="13"/>
+    <col min="10497" max="10497" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10498" max="10752" width="8.7265625" style="13"/>
+    <col min="10753" max="10753" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10754" max="11008" width="8.7265625" style="13"/>
+    <col min="11009" max="11009" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="11010" max="11264" width="8.7265625" style="13"/>
+    <col min="11265" max="11265" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="11266" max="11520" width="8.7265625" style="13"/>
+    <col min="11521" max="11521" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="11522" max="11776" width="8.7265625" style="13"/>
+    <col min="11777" max="11777" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="11778" max="12032" width="8.7265625" style="13"/>
+    <col min="12033" max="12033" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="12034" max="12288" width="8.7265625" style="13"/>
+    <col min="12289" max="12289" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="12290" max="12544" width="8.7265625" style="13"/>
+    <col min="12545" max="12545" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="12546" max="12800" width="8.7265625" style="13"/>
+    <col min="12801" max="12801" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="12802" max="13056" width="8.7265625" style="13"/>
+    <col min="13057" max="13057" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="13058" max="13312" width="8.7265625" style="13"/>
+    <col min="13313" max="13313" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="13314" max="13568" width="8.7265625" style="13"/>
+    <col min="13569" max="13569" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="13570" max="13824" width="8.7265625" style="13"/>
+    <col min="13825" max="13825" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="13826" max="14080" width="8.7265625" style="13"/>
+    <col min="14081" max="14081" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="14082" max="14336" width="8.7265625" style="13"/>
+    <col min="14337" max="14337" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="14338" max="14592" width="8.7265625" style="13"/>
+    <col min="14593" max="14593" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="14594" max="14848" width="8.7265625" style="13"/>
+    <col min="14849" max="14849" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="14850" max="15104" width="8.7265625" style="13"/>
+    <col min="15105" max="15105" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="15106" max="15360" width="8.7265625" style="13"/>
+    <col min="15361" max="15361" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="15362" max="15616" width="8.7265625" style="13"/>
+    <col min="15617" max="15617" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="15618" max="15872" width="8.7265625" style="13"/>
+    <col min="15873" max="15873" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="15874" max="16128" width="8.7265625" style="13"/>
+    <col min="16129" max="16129" width="31.1328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="16130" max="16384" width="8.7265625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.6">
       <c r="A1" s="12" t="s">
         <v>127</v>
       </c>
@@ -26251,7 +26255,7 @@
         <v>6_2_3_MR</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.6">
       <c r="A2" s="13" t="s">
         <v>128</v>
       </c>
@@ -26396,7 +26400,7 @@
         <v>&lt;0,068</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.6">
       <c r="A3" s="13" t="s">
         <v>129</v>
       </c>
@@ -26541,7 +26545,7 @@
         <v>&lt;0,075</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.6">
       <c r="A4" s="13" t="s">
         <v>130</v>
       </c>
@@ -26686,7 +26690,7 @@
         <v>&lt;1,673</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.6">
       <c r="A5" s="13" t="s">
         <v>131</v>
       </c>
@@ -26831,7 +26835,7 @@
         <v>&lt;0,133</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.6">
       <c r="A6" s="13" t="s">
         <v>132</v>
       </c>
@@ -26976,7 +26980,7 @@
         <v>&lt;36,874</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.6">
       <c r="A7" s="13" t="s">
         <v>133</v>
       </c>
@@ -27121,7 +27125,7 @@
         <v>&lt;6,857</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.6">
       <c r="A8" s="13" t="s">
         <v>134</v>
       </c>
@@ -27266,7 +27270,7 @@
         <v>&lt;0,077</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.6">
       <c r="A9" s="13" t="s">
         <v>135</v>
       </c>
@@ -27411,7 +27415,7 @@
         <v>&lt;0,117</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.6">
       <c r="A10" s="13" t="s">
         <v>136</v>
       </c>
@@ -27556,7 +27560,7 @@
         <v>&lt;0,959</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.6">
       <c r="A11" s="13" t="s">
         <v>137</v>
       </c>
@@ -27701,7 +27705,7 @@
         <v>&lt;0,039</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.6">
       <c r="A12" s="13" t="s">
         <v>138</v>
       </c>
@@ -27846,7 +27850,7 @@
         <v>&lt;1,497</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.6">
       <c r="A13" s="13" t="s">
         <v>139</v>
       </c>
@@ -27991,7 +27995,7 @@
         <v>&lt;0,069</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.6">
       <c r="A14" s="13" t="s">
         <v>140</v>
       </c>
@@ -28136,7 +28140,7 @@
         <v>&lt;0,102</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.6">
       <c r="A15" s="13" t="s">
         <v>141</v>
       </c>
@@ -28281,7 +28285,7 @@
         <v>&lt;2,915</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.6">
       <c r="A16" s="13" t="s">
         <v>142</v>
       </c>
@@ -28426,7 +28430,7 @@
         <v>&lt;0,057</v>
       </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.6">
       <c r="A17" s="13" t="s">
         <v>143</v>
       </c>
@@ -28571,7 +28575,7 @@
         <v>&lt;0,084</v>
       </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.6">
       <c r="A18" s="13" t="s">
         <v>144</v>
       </c>
@@ -28716,7 +28720,7 @@
         <v>&lt;0,063</v>
       </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.6">
       <c r="A19" s="13" t="s">
         <v>145</v>
       </c>
@@ -28861,7 +28865,7 @@
         <v>&lt;0,091</v>
       </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.6">
       <c r="A20" s="13" t="s">
         <v>146</v>
       </c>
@@ -29006,7 +29010,7 @@
         <v>&lt;0,137</v>
       </c>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.6">
       <c r="A21" s="13" t="s">
         <v>147</v>
       </c>
@@ -29151,7 +29155,7 @@
         <v>&lt;3,368</v>
       </c>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.6">
       <c r="A22" s="13" t="s">
         <v>148</v>
       </c>
@@ -29296,7 +29300,7 @@
         <v>&lt;0,113</v>
       </c>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.6">
       <c r="A23" s="13" t="s">
         <v>149</v>
       </c>
@@ -29441,7 +29445,7 @@
         <v>&lt;13,511</v>
       </c>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.6">
       <c r="A24" s="13" t="s">
         <v>150</v>
       </c>
@@ -29586,7 +29590,7 @@
         <v>&lt;3,866</v>
       </c>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.6">
       <c r="A25" s="13" t="s">
         <v>151</v>
       </c>
@@ -29731,7 +29735,7 @@
         <v>&lt;0,649</v>
       </c>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.6">
       <c r="A26" s="13" t="s">
         <v>152</v>
       </c>
@@ -29876,7 +29880,7 @@
         <v>&lt;0,388</v>
       </c>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.6">
       <c r="A27" s="13" t="s">
         <v>153</v>
       </c>
@@ -30021,7 +30025,7 @@
         <v>&lt;0,109</v>
       </c>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.6">
       <c r="A28" s="13" t="s">
         <v>154</v>
       </c>
@@ -30166,7 +30170,7 @@
         <v>&lt;0,221</v>
       </c>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.6">
       <c r="A29" s="13" t="s">
         <v>155</v>
       </c>

</xml_diff>